<commit_message>
, added regressions, clustering, scalars, vextors, ms and tensors
</commit_message>
<xml_diff>
--- a/investing/sp500_dfs/commodities_ohlc.xlsx
+++ b/investing/sp500_dfs/commodities_ohlc.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG599"/>
+  <dimension ref="A1:AG615"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -60907,7 +60907,7 @@
         <v>2412.199951171875</v>
       </c>
       <c r="G599" t="n">
-        <v>7</v>
+        <v>213</v>
       </c>
       <c r="H599" t="n">
         <v>0.01474360414002291</v>
@@ -60931,7 +60931,7 @@
         <v>1084.599975585938</v>
       </c>
       <c r="O599" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P599" t="n">
         <v>0</v>
@@ -60955,7 +60955,7 @@
         <v>5.057000160217285</v>
       </c>
       <c r="W599" t="n">
-        <v>1150</v>
+        <v>790</v>
       </c>
       <c r="X599" t="n">
         <v>0.04224052118254837</v>
@@ -60979,13 +60979,1629 @@
         <v>80.05999755859375</v>
       </c>
       <c r="AE599" t="n">
-        <v>230277</v>
+        <v>94152</v>
       </c>
       <c r="AF599" t="n">
         <v>0.0144303720208663</v>
       </c>
       <c r="AG599" t="n">
         <v>0.008566393659663444</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="2" t="n">
+        <v>45432</v>
+      </c>
+      <c r="B600" t="n">
+        <v>2415.800048828125</v>
+      </c>
+      <c r="C600" t="n">
+        <v>2435.800048828125</v>
+      </c>
+      <c r="D600" t="n">
+        <v>2409.699951171875</v>
+      </c>
+      <c r="E600" t="n">
+        <v>2433.89990234375</v>
+      </c>
+      <c r="F600" t="n">
+        <v>2433.89990234375</v>
+      </c>
+      <c r="G600" t="n">
+        <v>40</v>
+      </c>
+      <c r="H600" t="n">
+        <v>0.01083126454957893</v>
+      </c>
+      <c r="I600" t="n">
+        <v>0.007492281293894757</v>
+      </c>
+      <c r="J600" t="n">
+        <v>1059.699951171875</v>
+      </c>
+      <c r="K600" t="n">
+        <v>1059.699951171875</v>
+      </c>
+      <c r="L600" t="n">
+        <v>1059.699951171875</v>
+      </c>
+      <c r="M600" t="n">
+        <v>1059.699951171875</v>
+      </c>
+      <c r="N600" t="n">
+        <v>1059.699951171875</v>
+      </c>
+      <c r="O600" t="n">
+        <v>0</v>
+      </c>
+      <c r="P600" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q600" t="n">
+        <v>0</v>
+      </c>
+      <c r="R600" t="n">
+        <v>5.191999912261963</v>
+      </c>
+      <c r="S600" t="n">
+        <v>5.198500156402588</v>
+      </c>
+      <c r="T600" t="n">
+        <v>5.028999805450439</v>
+      </c>
+      <c r="U600" t="n">
+        <v>5.087500095367432</v>
+      </c>
+      <c r="V600" t="n">
+        <v>5.087500095367432</v>
+      </c>
+      <c r="W600" t="n">
+        <v>747</v>
+      </c>
+      <c r="X600" t="n">
+        <v>0.03370458490939762</v>
+      </c>
+      <c r="Y600" t="n">
+        <v>-0.02012708371734246</v>
+      </c>
+      <c r="Z600" t="n">
+        <v>80.01000213623047</v>
+      </c>
+      <c r="AA600" t="n">
+        <v>80.59999847412109</v>
+      </c>
+      <c r="AB600" t="n">
+        <v>79.16999816894531</v>
+      </c>
+      <c r="AC600" t="n">
+        <v>79.80000305175781</v>
+      </c>
+      <c r="AD600" t="n">
+        <v>79.80000305175781</v>
+      </c>
+      <c r="AE600" t="n">
+        <v>85072</v>
+      </c>
+      <c r="AF600" t="n">
+        <v>0.01806240164518159</v>
+      </c>
+      <c r="AG600" t="n">
+        <v>-0.0026246604032718</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" s="2" t="n">
+        <v>45433</v>
+      </c>
+      <c r="B601" t="n">
+        <v>2429.5</v>
+      </c>
+      <c r="C601" t="n">
+        <v>2429.5</v>
+      </c>
+      <c r="D601" t="n">
+        <v>2421</v>
+      </c>
+      <c r="E601" t="n">
+        <v>2421.699951171875</v>
+      </c>
+      <c r="F601" t="n">
+        <v>2421.699951171875</v>
+      </c>
+      <c r="G601" t="n">
+        <v>6</v>
+      </c>
+      <c r="H601" t="n">
+        <v>0.003510945890128046</v>
+      </c>
+      <c r="I601" t="n">
+        <v>-0.003210557245575221</v>
+      </c>
+      <c r="J601" t="n">
+        <v>1056.699951171875</v>
+      </c>
+      <c r="K601" t="n">
+        <v>1056.699951171875</v>
+      </c>
+      <c r="L601" t="n">
+        <v>1056.699951171875</v>
+      </c>
+      <c r="M601" t="n">
+        <v>1056.699951171875</v>
+      </c>
+      <c r="N601" t="n">
+        <v>1056.699951171875</v>
+      </c>
+      <c r="O601" t="n">
+        <v>0</v>
+      </c>
+      <c r="P601" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q601" t="n">
+        <v>0</v>
+      </c>
+      <c r="R601" t="n">
+        <v>5.057499885559082</v>
+      </c>
+      <c r="S601" t="n">
+        <v>5.161499977111816</v>
+      </c>
+      <c r="T601" t="n">
+        <v>5.057499885559082</v>
+      </c>
+      <c r="U601" t="n">
+        <v>5.11899995803833</v>
+      </c>
+      <c r="V601" t="n">
+        <v>5.11899995803833</v>
+      </c>
+      <c r="W601" t="n">
+        <v>568</v>
+      </c>
+      <c r="X601" t="n">
+        <v>0.02056353809313783</v>
+      </c>
+      <c r="Y601" t="n">
+        <v>0.01216017278712197</v>
+      </c>
+      <c r="Z601" t="n">
+        <v>79.69999694824219</v>
+      </c>
+      <c r="AA601" t="n">
+        <v>79.72000122070312</v>
+      </c>
+      <c r="AB601" t="n">
+        <v>78.08000183105469</v>
+      </c>
+      <c r="AC601" t="n">
+        <v>79.26000213623047</v>
+      </c>
+      <c r="AD601" t="n">
+        <v>79.26000213623047</v>
+      </c>
+      <c r="AE601" t="n">
+        <v>371672</v>
+      </c>
+      <c r="AF601" t="n">
+        <v>0.02100409005108607</v>
+      </c>
+      <c r="AG601" t="n">
+        <v>-0.005520637752313277</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B602" t="n">
+        <v>2417.5</v>
+      </c>
+      <c r="C602" t="n">
+        <v>2417.60009765625</v>
+      </c>
+      <c r="D602" t="n">
+        <v>2375.800048828125</v>
+      </c>
+      <c r="E602" t="n">
+        <v>2389.199951171875</v>
+      </c>
+      <c r="F602" t="n">
+        <v>2389.199951171875</v>
+      </c>
+      <c r="G602" t="n">
+        <v>180</v>
+      </c>
+      <c r="H602" t="n">
+        <v>0.01759409376590554</v>
+      </c>
+      <c r="I602" t="n">
+        <v>-0.01170632836737332</v>
+      </c>
+      <c r="J602" t="n">
+        <v>1044.099975585938</v>
+      </c>
+      <c r="K602" t="n">
+        <v>1044.099975585938</v>
+      </c>
+      <c r="L602" t="n">
+        <v>1044.099975585938</v>
+      </c>
+      <c r="M602" t="n">
+        <v>1044.099975585938</v>
+      </c>
+      <c r="N602" t="n">
+        <v>1044.099975585938</v>
+      </c>
+      <c r="O602" t="n">
+        <v>0</v>
+      </c>
+      <c r="P602" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q602" t="n">
+        <v>0</v>
+      </c>
+      <c r="R602" t="n">
+        <v>5.074999809265137</v>
+      </c>
+      <c r="S602" t="n">
+        <v>5.074999809265137</v>
+      </c>
+      <c r="T602" t="n">
+        <v>4.839000225067139</v>
+      </c>
+      <c r="U602" t="n">
+        <v>4.867499828338623</v>
+      </c>
+      <c r="V602" t="n">
+        <v>4.867499828338623</v>
+      </c>
+      <c r="W602" t="n">
+        <v>976</v>
+      </c>
+      <c r="X602" t="n">
+        <v>0.04877031891328826</v>
+      </c>
+      <c r="Y602" t="n">
+        <v>-0.04088669728572065</v>
+      </c>
+      <c r="Z602" t="n">
+        <v>78.20999908447266</v>
+      </c>
+      <c r="AA602" t="n">
+        <v>78.41000366210938</v>
+      </c>
+      <c r="AB602" t="n">
+        <v>77.25</v>
+      </c>
+      <c r="AC602" t="n">
+        <v>77.56999969482422</v>
+      </c>
+      <c r="AD602" t="n">
+        <v>77.56999969482422</v>
+      </c>
+      <c r="AE602" t="n">
+        <v>314145</v>
+      </c>
+      <c r="AF602" t="n">
+        <v>0.01501622863572006</v>
+      </c>
+      <c r="AG602" t="n">
+        <v>-0.008183089082473843</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="2" t="n">
+        <v>45435</v>
+      </c>
+      <c r="B603" t="n">
+        <v>2371.199951171875</v>
+      </c>
+      <c r="C603" t="n">
+        <v>2371.199951171875</v>
+      </c>
+      <c r="D603" t="n">
+        <v>2335</v>
+      </c>
+      <c r="E603" t="n">
+        <v>2335</v>
+      </c>
+      <c r="F603" t="n">
+        <v>2335</v>
+      </c>
+      <c r="G603" t="n">
+        <v>365</v>
+      </c>
+      <c r="H603" t="n">
+        <v>0.01550319108003212</v>
+      </c>
+      <c r="I603" t="n">
+        <v>-0.01526651143611257</v>
+      </c>
+      <c r="J603" t="n">
+        <v>1025.699951171875</v>
+      </c>
+      <c r="K603" t="n">
+        <v>1025.699951171875</v>
+      </c>
+      <c r="L603" t="n">
+        <v>1025.699951171875</v>
+      </c>
+      <c r="M603" t="n">
+        <v>1025.699951171875</v>
+      </c>
+      <c r="N603" t="n">
+        <v>1025.699951171875</v>
+      </c>
+      <c r="O603" t="n">
+        <v>2</v>
+      </c>
+      <c r="P603" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q603" t="n">
+        <v>0</v>
+      </c>
+      <c r="R603" t="n">
+        <v>4.809999942779541</v>
+      </c>
+      <c r="S603" t="n">
+        <v>4.848000049591064</v>
+      </c>
+      <c r="T603" t="n">
+        <v>4.803500175476074</v>
+      </c>
+      <c r="U603" t="n">
+        <v>4.816500186920166</v>
+      </c>
+      <c r="V603" t="n">
+        <v>4.816500186920166</v>
+      </c>
+      <c r="W603" t="n">
+        <v>713</v>
+      </c>
+      <c r="X603" t="n">
+        <v>0.009264051730898471</v>
+      </c>
+      <c r="Y603" t="n">
+        <v>0.001351402124314522</v>
+      </c>
+      <c r="Z603" t="n">
+        <v>77.29000091552734</v>
+      </c>
+      <c r="AA603" t="n">
+        <v>78.66000366210938</v>
+      </c>
+      <c r="AB603" t="n">
+        <v>76.43000030517578</v>
+      </c>
+      <c r="AC603" t="n">
+        <v>76.87000274658203</v>
+      </c>
+      <c r="AD603" t="n">
+        <v>76.87000274658203</v>
+      </c>
+      <c r="AE603" t="n">
+        <v>330273</v>
+      </c>
+      <c r="AF603" t="n">
+        <v>0.02917706853368388</v>
+      </c>
+      <c r="AG603" t="n">
+        <v>-0.005434055685991537</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="2" t="n">
+        <v>45436</v>
+      </c>
+      <c r="B604" t="n">
+        <v>2342.60009765625</v>
+      </c>
+      <c r="C604" t="n">
+        <v>2345.39990234375</v>
+      </c>
+      <c r="D604" t="n">
+        <v>2332.5</v>
+      </c>
+      <c r="E604" t="n">
+        <v>2332.5</v>
+      </c>
+      <c r="F604" t="n">
+        <v>2332.5</v>
+      </c>
+      <c r="G604" t="n">
+        <v>25</v>
+      </c>
+      <c r="H604" t="n">
+        <v>0.005530504756162916</v>
+      </c>
+      <c r="I604" t="n">
+        <v>-0.004311490324940674</v>
+      </c>
+      <c r="J604" t="n">
+        <v>1034.800048828125</v>
+      </c>
+      <c r="K604" t="n">
+        <v>1034.800048828125</v>
+      </c>
+      <c r="L604" t="n">
+        <v>1034.800048828125</v>
+      </c>
+      <c r="M604" t="n">
+        <v>1034.800048828125</v>
+      </c>
+      <c r="N604" t="n">
+        <v>1034.800048828125</v>
+      </c>
+      <c r="O604" t="n">
+        <v>2</v>
+      </c>
+      <c r="P604" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q604" t="n">
+        <v>0</v>
+      </c>
+      <c r="R604" t="n">
+        <v>4.815999984741211</v>
+      </c>
+      <c r="S604" t="n">
+        <v>4.824999809265137</v>
+      </c>
+      <c r="T604" t="n">
+        <v>4.772500038146973</v>
+      </c>
+      <c r="U604" t="n">
+        <v>4.778500080108643</v>
+      </c>
+      <c r="V604" t="n">
+        <v>4.778500080108643</v>
+      </c>
+      <c r="W604" t="n">
+        <v>689</v>
+      </c>
+      <c r="X604" t="n">
+        <v>0.0110004757880627</v>
+      </c>
+      <c r="Y604" t="n">
+        <v>-0.007786525072961234</v>
+      </c>
+      <c r="Z604" t="n">
+        <v>77.04000091552734</v>
+      </c>
+      <c r="AA604" t="n">
+        <v>78.05000305175781</v>
+      </c>
+      <c r="AB604" t="n">
+        <v>76.15000152587891</v>
+      </c>
+      <c r="AC604" t="n">
+        <v>77.72000122070312</v>
+      </c>
+      <c r="AD604" t="n">
+        <v>77.72000122070312</v>
+      </c>
+      <c r="AE604" t="n">
+        <v>299075</v>
+      </c>
+      <c r="AF604" t="n">
+        <v>0.02495077462648779</v>
+      </c>
+      <c r="AG604" t="n">
+        <v>0.008826587449309437</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" s="2" t="n">
+        <v>45440</v>
+      </c>
+      <c r="B605" t="n">
+        <v>2336.89990234375</v>
+      </c>
+      <c r="C605" t="n">
+        <v>2359.699951171875</v>
+      </c>
+      <c r="D605" t="n">
+        <v>2336.89990234375</v>
+      </c>
+      <c r="E605" t="n">
+        <v>2355.199951171875</v>
+      </c>
+      <c r="F605" t="n">
+        <v>2355.199951171875</v>
+      </c>
+      <c r="G605" t="n">
+        <v>26</v>
+      </c>
+      <c r="H605" t="n">
+        <v>0.009756536343408683</v>
+      </c>
+      <c r="I605" t="n">
+        <v>0.007830908294262544</v>
+      </c>
+      <c r="J605" t="n">
+        <v>1061.699951171875</v>
+      </c>
+      <c r="K605" t="n">
+        <v>1061.699951171875</v>
+      </c>
+      <c r="L605" t="n">
+        <v>1061.699951171875</v>
+      </c>
+      <c r="M605" t="n">
+        <v>1061.699951171875</v>
+      </c>
+      <c r="N605" t="n">
+        <v>1061.699951171875</v>
+      </c>
+      <c r="O605" t="n">
+        <v>2</v>
+      </c>
+      <c r="P605" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q605" t="n">
+        <v>0</v>
+      </c>
+      <c r="R605" t="n">
+        <v>4.863500118255615</v>
+      </c>
+      <c r="S605" t="n">
+        <v>4.89900016784668</v>
+      </c>
+      <c r="T605" t="n">
+        <v>4.860000133514404</v>
+      </c>
+      <c r="U605" t="n">
+        <v>4.875500202178955</v>
+      </c>
+      <c r="V605" t="n">
+        <v>4.875500202178955</v>
+      </c>
+      <c r="W605" t="n">
+        <v>461</v>
+      </c>
+      <c r="X605" t="n">
+        <v>0.008024698201823579</v>
+      </c>
+      <c r="Y605" t="n">
+        <v>0.002467376093668914</v>
+      </c>
+      <c r="Z605" t="n">
+        <v>77.80999755859375</v>
+      </c>
+      <c r="AA605" t="n">
+        <v>80.29000091552734</v>
+      </c>
+      <c r="AB605" t="n">
+        <v>77.69000244140625</v>
+      </c>
+      <c r="AC605" t="n">
+        <v>79.83000183105469</v>
+      </c>
+      <c r="AD605" t="n">
+        <v>79.83000183105469</v>
+      </c>
+      <c r="AE605" t="n">
+        <v>334074</v>
+      </c>
+      <c r="AF605" t="n">
+        <v>0.03346631989208664</v>
+      </c>
+      <c r="AG605" t="n">
+        <v>0.02596072915874083</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B606" t="n">
+        <v>2340.300048828125</v>
+      </c>
+      <c r="C606" t="n">
+        <v>2340.300048828125</v>
+      </c>
+      <c r="D606" t="n">
+        <v>2340.300048828125</v>
+      </c>
+      <c r="E606" t="n">
+        <v>2340.300048828125</v>
+      </c>
+      <c r="F606" t="n">
+        <v>2340.300048828125</v>
+      </c>
+      <c r="G606" t="n">
+        <v>119317</v>
+      </c>
+      <c r="H606" t="n">
+        <v>0</v>
+      </c>
+      <c r="I606" t="n">
+        <v>0</v>
+      </c>
+      <c r="J606" t="n">
+        <v>1042.699951171875</v>
+      </c>
+      <c r="K606" t="n">
+        <v>1042.699951171875</v>
+      </c>
+      <c r="L606" t="n">
+        <v>1042.699951171875</v>
+      </c>
+      <c r="M606" t="n">
+        <v>1042.699951171875</v>
+      </c>
+      <c r="N606" t="n">
+        <v>1042.699951171875</v>
+      </c>
+      <c r="O606" t="n">
+        <v>59</v>
+      </c>
+      <c r="P606" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q606" t="n">
+        <v>0</v>
+      </c>
+      <c r="R606" t="n">
+        <v>4.802000045776367</v>
+      </c>
+      <c r="S606" t="n">
+        <v>4.805500030517578</v>
+      </c>
+      <c r="T606" t="n">
+        <v>4.796000003814697</v>
+      </c>
+      <c r="U606" t="n">
+        <v>4.805500030517578</v>
+      </c>
+      <c r="V606" t="n">
+        <v>4.805500030517578</v>
+      </c>
+      <c r="W606" t="n">
+        <v>1059</v>
+      </c>
+      <c r="X606" t="n">
+        <v>0.001980822913954257</v>
+      </c>
+      <c r="Y606" t="n">
+        <v>0.0007288597892224874</v>
+      </c>
+      <c r="Z606" t="n">
+        <v>80.26000213623047</v>
+      </c>
+      <c r="AA606" t="n">
+        <v>80.62000274658203</v>
+      </c>
+      <c r="AB606" t="n">
+        <v>78.98999786376953</v>
+      </c>
+      <c r="AC606" t="n">
+        <v>79.23000335693359</v>
+      </c>
+      <c r="AD606" t="n">
+        <v>79.23000335693359</v>
+      </c>
+      <c r="AE606" t="n">
+        <v>259594</v>
+      </c>
+      <c r="AF606" t="n">
+        <v>0.02063558585763853</v>
+      </c>
+      <c r="AG606" t="n">
+        <v>-0.01283327625071068</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="2" t="n">
+        <v>45442</v>
+      </c>
+      <c r="B607" t="n">
+        <v>2336.89990234375</v>
+      </c>
+      <c r="C607" t="n">
+        <v>2349.5</v>
+      </c>
+      <c r="D607" t="n">
+        <v>2320.800048828125</v>
+      </c>
+      <c r="E607" t="n">
+        <v>2342.89990234375</v>
+      </c>
+      <c r="F607" t="n">
+        <v>2342.89990234375</v>
+      </c>
+      <c r="G607" t="n">
+        <v>32587</v>
+      </c>
+      <c r="H607" t="n">
+        <v>0.01236640407103011</v>
+      </c>
+      <c r="I607" t="n">
+        <v>0.002567504065528187</v>
+      </c>
+      <c r="J607" t="n">
+        <v>1034.800048828125</v>
+      </c>
+      <c r="K607" t="n">
+        <v>1038.300048828125</v>
+      </c>
+      <c r="L607" t="n">
+        <v>1032.699951171875</v>
+      </c>
+      <c r="M607" t="n">
+        <v>1032.900024414062</v>
+      </c>
+      <c r="N607" t="n">
+        <v>1032.900024414062</v>
+      </c>
+      <c r="O607" t="n">
+        <v>11</v>
+      </c>
+      <c r="P607" t="n">
+        <v>0.005422773236209789</v>
+      </c>
+      <c r="Q607" t="n">
+        <v>-0.001836127101283201</v>
+      </c>
+      <c r="R607" t="n">
+        <v>4.775499820709229</v>
+      </c>
+      <c r="S607" t="n">
+        <v>4.785500049591064</v>
+      </c>
+      <c r="T607" t="n">
+        <v>4.642499923706055</v>
+      </c>
+      <c r="U607" t="n">
+        <v>4.671999931335449</v>
+      </c>
+      <c r="V607" t="n">
+        <v>4.671999931335449</v>
+      </c>
+      <c r="W607" t="n">
+        <v>1170</v>
+      </c>
+      <c r="X607" t="n">
+        <v>0.03080239703501263</v>
+      </c>
+      <c r="Y607" t="n">
+        <v>-0.02167310088149226</v>
+      </c>
+      <c r="Z607" t="n">
+        <v>79.27999877929688</v>
+      </c>
+      <c r="AA607" t="n">
+        <v>79.41999816894531</v>
+      </c>
+      <c r="AB607" t="n">
+        <v>77.62999725341797</v>
+      </c>
+      <c r="AC607" t="n">
+        <v>77.91000366210938</v>
+      </c>
+      <c r="AD607" t="n">
+        <v>77.91000366210938</v>
+      </c>
+      <c r="AE607" t="n">
+        <v>373779</v>
+      </c>
+      <c r="AF607" t="n">
+        <v>0.02305810870614879</v>
+      </c>
+      <c r="AG607" t="n">
+        <v>-0.01728046339911473</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" s="2" t="n">
+        <v>45443</v>
+      </c>
+      <c r="B608" t="n">
+        <v>2344.10009765625</v>
+      </c>
+      <c r="C608" t="n">
+        <v>2354</v>
+      </c>
+      <c r="D608" t="n">
+        <v>2319</v>
+      </c>
+      <c r="E608" t="n">
+        <v>2322.89990234375</v>
+      </c>
+      <c r="F608" t="n">
+        <v>2322.89990234375</v>
+      </c>
+      <c r="G608" t="n">
+        <v>941</v>
+      </c>
+      <c r="H608" t="n">
+        <v>0.01509271237602415</v>
+      </c>
+      <c r="I608" t="n">
+        <v>-0.009044065709351332</v>
+      </c>
+      <c r="J608" t="n">
+        <v>1028</v>
+      </c>
+      <c r="K608" t="n">
+        <v>1037.699951171875</v>
+      </c>
+      <c r="L608" t="n">
+        <v>1028</v>
+      </c>
+      <c r="M608" t="n">
+        <v>1037.699951171875</v>
+      </c>
+      <c r="N608" t="n">
+        <v>1037.699951171875</v>
+      </c>
+      <c r="O608" t="n">
+        <v>2</v>
+      </c>
+      <c r="P608" t="n">
+        <v>0.00943575016719358</v>
+      </c>
+      <c r="Q608" t="n">
+        <v>0.00943575016719358</v>
+      </c>
+      <c r="R608" t="n">
+        <v>4.638500213623047</v>
+      </c>
+      <c r="S608" t="n">
+        <v>4.651500225067139</v>
+      </c>
+      <c r="T608" t="n">
+        <v>4.583499908447266</v>
+      </c>
+      <c r="U608" t="n">
+        <v>4.610000133514404</v>
+      </c>
+      <c r="V608" t="n">
+        <v>4.610000133514404</v>
+      </c>
+      <c r="W608" t="n">
+        <v>615</v>
+      </c>
+      <c r="X608" t="n">
+        <v>0.01483589352637497</v>
+      </c>
+      <c r="Y608" t="n">
+        <v>-0.006144244647211451</v>
+      </c>
+      <c r="Z608" t="n">
+        <v>77.91000366210938</v>
+      </c>
+      <c r="AA608" t="n">
+        <v>78.62000274658203</v>
+      </c>
+      <c r="AB608" t="n">
+        <v>76.66999816894531</v>
+      </c>
+      <c r="AC608" t="n">
+        <v>76.98999786376953</v>
+      </c>
+      <c r="AD608" t="n">
+        <v>76.98999786376953</v>
+      </c>
+      <c r="AE608" t="n">
+        <v>345120</v>
+      </c>
+      <c r="AF608" t="n">
+        <v>0.02543373710978587</v>
+      </c>
+      <c r="AG608" t="n">
+        <v>-0.01180857085220852</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="2" t="n">
+        <v>45446</v>
+      </c>
+      <c r="B609" t="n">
+        <v>2322.60009765625</v>
+      </c>
+      <c r="C609" t="n">
+        <v>2347.5</v>
+      </c>
+      <c r="D609" t="n">
+        <v>2312</v>
+      </c>
+      <c r="E609" t="n">
+        <v>2346.60009765625</v>
+      </c>
+      <c r="F609" t="n">
+        <v>2346.60009765625</v>
+      </c>
+      <c r="G609" t="n">
+        <v>781</v>
+      </c>
+      <c r="H609" t="n">
+        <v>0.01535467128027682</v>
+      </c>
+      <c r="I609" t="n">
+        <v>0.01033324678846718</v>
+      </c>
+      <c r="J609" t="n">
+        <v>1018.5</v>
+      </c>
+      <c r="K609" t="n">
+        <v>1018.5</v>
+      </c>
+      <c r="L609" t="n">
+        <v>1018.5</v>
+      </c>
+      <c r="M609" t="n">
+        <v>1018.5</v>
+      </c>
+      <c r="N609" t="n">
+        <v>1018.5</v>
+      </c>
+      <c r="O609" t="n">
+        <v>2</v>
+      </c>
+      <c r="P609" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q609" t="n">
+        <v>0</v>
+      </c>
+      <c r="R609" t="n">
+        <v>4.684000015258789</v>
+      </c>
+      <c r="S609" t="n">
+        <v>4.684000015258789</v>
+      </c>
+      <c r="T609" t="n">
+        <v>4.663000106811523</v>
+      </c>
+      <c r="U609" t="n">
+        <v>4.677000045776367</v>
+      </c>
+      <c r="V609" t="n">
+        <v>4.677000045776367</v>
+      </c>
+      <c r="W609" t="n">
+        <v>488</v>
+      </c>
+      <c r="X609" t="n">
+        <v>0.004503518757503308</v>
+      </c>
+      <c r="Y609" t="n">
+        <v>-0.001494442668577816</v>
+      </c>
+      <c r="Z609" t="n">
+        <v>76.97000122070312</v>
+      </c>
+      <c r="AA609" t="n">
+        <v>77.51999664306641</v>
+      </c>
+      <c r="AB609" t="n">
+        <v>73.98000335693359</v>
+      </c>
+      <c r="AC609" t="n">
+        <v>74.22000122070312</v>
+      </c>
+      <c r="AD609" t="n">
+        <v>74.22000122070312</v>
+      </c>
+      <c r="AE609" t="n">
+        <v>443271</v>
+      </c>
+      <c r="AF609" t="n">
+        <v>0.04785067755476163</v>
+      </c>
+      <c r="AG609" t="n">
+        <v>-0.03572820522783511</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="2" t="n">
+        <v>45447</v>
+      </c>
+      <c r="B610" t="n">
+        <v>2347.5</v>
+      </c>
+      <c r="C610" t="n">
+        <v>2347.699951171875</v>
+      </c>
+      <c r="D610" t="n">
+        <v>2313.89990234375</v>
+      </c>
+      <c r="E610" t="n">
+        <v>2325.5</v>
+      </c>
+      <c r="F610" t="n">
+        <v>2325.5</v>
+      </c>
+      <c r="G610" t="n">
+        <v>890</v>
+      </c>
+      <c r="H610" t="n">
+        <v>0.01460739455232654</v>
+      </c>
+      <c r="I610" t="n">
+        <v>-0.009371671991480299</v>
+      </c>
+      <c r="J610" t="n">
+        <v>991.5999755859375</v>
+      </c>
+      <c r="K610" t="n">
+        <v>991.5999755859375</v>
+      </c>
+      <c r="L610" t="n">
+        <v>991.5999755859375</v>
+      </c>
+      <c r="M610" t="n">
+        <v>991.5999755859375</v>
+      </c>
+      <c r="N610" t="n">
+        <v>991.5999755859375</v>
+      </c>
+      <c r="O610" t="n">
+        <v>2</v>
+      </c>
+      <c r="P610" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q610" t="n">
+        <v>0</v>
+      </c>
+      <c r="R610" t="n">
+        <v>4.685999870300293</v>
+      </c>
+      <c r="S610" t="n">
+        <v>4.685999870300293</v>
+      </c>
+      <c r="T610" t="n">
+        <v>4.54449987411499</v>
+      </c>
+      <c r="U610" t="n">
+        <v>4.547999858856201</v>
+      </c>
+      <c r="V610" t="n">
+        <v>4.547999858856201</v>
+      </c>
+      <c r="W610" t="n">
+        <v>593</v>
+      </c>
+      <c r="X610" t="n">
+        <v>0.03113653869620997</v>
+      </c>
+      <c r="Y610" t="n">
+        <v>-0.02944942707291376</v>
+      </c>
+      <c r="Z610" t="n">
+        <v>74.01999664306641</v>
+      </c>
+      <c r="AA610" t="n">
+        <v>74.12999725341797</v>
+      </c>
+      <c r="AB610" t="n">
+        <v>72.48000335693359</v>
+      </c>
+      <c r="AC610" t="n">
+        <v>73.25</v>
+      </c>
+      <c r="AD610" t="n">
+        <v>73.25</v>
+      </c>
+      <c r="AE610" t="n">
+        <v>408721</v>
+      </c>
+      <c r="AF610" t="n">
+        <v>0.02276481539823954</v>
+      </c>
+      <c r="AG610" t="n">
+        <v>-0.01040254901360541</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" s="2" t="n">
+        <v>45448</v>
+      </c>
+      <c r="B611" t="n">
+        <v>2326.39990234375</v>
+      </c>
+      <c r="C611" t="n">
+        <v>2354.300048828125</v>
+      </c>
+      <c r="D611" t="n">
+        <v>2326.199951171875</v>
+      </c>
+      <c r="E611" t="n">
+        <v>2354.10009765625</v>
+      </c>
+      <c r="F611" t="n">
+        <v>2354.10009765625</v>
+      </c>
+      <c r="G611" t="n">
+        <v>295</v>
+      </c>
+      <c r="H611" t="n">
+        <v>0.01207982901129972</v>
+      </c>
+      <c r="I611" t="n">
+        <v>0.0119068932579447</v>
+      </c>
+      <c r="J611" t="n">
+        <v>996</v>
+      </c>
+      <c r="K611" t="n">
+        <v>996</v>
+      </c>
+      <c r="L611" t="n">
+        <v>996</v>
+      </c>
+      <c r="M611" t="n">
+        <v>996</v>
+      </c>
+      <c r="N611" t="n">
+        <v>996</v>
+      </c>
+      <c r="O611" t="n">
+        <v>2</v>
+      </c>
+      <c r="P611" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q611" t="n">
+        <v>0</v>
+      </c>
+      <c r="R611" t="n">
+        <v>4.538000106811523</v>
+      </c>
+      <c r="S611" t="n">
+        <v>4.622499942779541</v>
+      </c>
+      <c r="T611" t="n">
+        <v>4.538000106811523</v>
+      </c>
+      <c r="U611" t="n">
+        <v>4.619500160217285</v>
+      </c>
+      <c r="V611" t="n">
+        <v>4.619500160217285</v>
+      </c>
+      <c r="W611" t="n">
+        <v>436</v>
+      </c>
+      <c r="X611" t="n">
+        <v>0.01862050109720879</v>
+      </c>
+      <c r="Y611" t="n">
+        <v>0.01795946484959981</v>
+      </c>
+      <c r="Z611" t="n">
+        <v>72.90000152587891</v>
+      </c>
+      <c r="AA611" t="n">
+        <v>74.33000183105469</v>
+      </c>
+      <c r="AB611" t="n">
+        <v>72.81999969482422</v>
+      </c>
+      <c r="AC611" t="n">
+        <v>74.06999969482422</v>
+      </c>
+      <c r="AD611" t="n">
+        <v>74.06999969482422</v>
+      </c>
+      <c r="AE611" t="n">
+        <v>307701</v>
+      </c>
+      <c r="AF611" t="n">
+        <v>0.02073609094422716</v>
+      </c>
+      <c r="AG611" t="n">
+        <v>0.01604935726277005</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="2" t="n">
+        <v>45449</v>
+      </c>
+      <c r="B612" t="n">
+        <v>2355</v>
+      </c>
+      <c r="C612" t="n">
+        <v>2375.800048828125</v>
+      </c>
+      <c r="D612" t="n">
+        <v>2355</v>
+      </c>
+      <c r="E612" t="n">
+        <v>2370.300048828125</v>
+      </c>
+      <c r="F612" t="n">
+        <v>2370.300048828125</v>
+      </c>
+      <c r="G612" t="n">
+        <v>179</v>
+      </c>
+      <c r="H612" t="n">
+        <v>0.008832292496019108</v>
+      </c>
+      <c r="I612" t="n">
+        <v>0.006496836020435244</v>
+      </c>
+      <c r="J612" t="n">
+        <v>1008.299987792969</v>
+      </c>
+      <c r="K612" t="n">
+        <v>1008.299987792969</v>
+      </c>
+      <c r="L612" t="n">
+        <v>1008.299987792969</v>
+      </c>
+      <c r="M612" t="n">
+        <v>1008.299987792969</v>
+      </c>
+      <c r="N612" t="n">
+        <v>1008.299987792969</v>
+      </c>
+      <c r="O612" t="n">
+        <v>2</v>
+      </c>
+      <c r="P612" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q612" t="n">
+        <v>0</v>
+      </c>
+      <c r="R612" t="n">
+        <v>4.661499977111816</v>
+      </c>
+      <c r="S612" t="n">
+        <v>4.690999984741211</v>
+      </c>
+      <c r="T612" t="n">
+        <v>4.650000095367432</v>
+      </c>
+      <c r="U612" t="n">
+        <v>4.690999984741211</v>
+      </c>
+      <c r="V612" t="n">
+        <v>4.690999984741211</v>
+      </c>
+      <c r="W612" t="n">
+        <v>376</v>
+      </c>
+      <c r="X612" t="n">
+        <v>0.008817180329657517</v>
+      </c>
+      <c r="Y612" t="n">
+        <v>0.006328436720849717</v>
+      </c>
+      <c r="Z612" t="n">
+        <v>74.30000305175781</v>
+      </c>
+      <c r="AA612" t="n">
+        <v>75.79000091552734</v>
+      </c>
+      <c r="AB612" t="n">
+        <v>74.05999755859375</v>
+      </c>
+      <c r="AC612" t="n">
+        <v>75.55000305175781</v>
+      </c>
+      <c r="AD612" t="n">
+        <v>75.55000305175781</v>
+      </c>
+      <c r="AE612" t="n">
+        <v>291082</v>
+      </c>
+      <c r="AF612" t="n">
+        <v>0.0233594843905426</v>
+      </c>
+      <c r="AG612" t="n">
+        <v>0.01682368706134834</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="2" t="n">
+        <v>45450</v>
+      </c>
+      <c r="B613" t="n">
+        <v>2379.89990234375</v>
+      </c>
+      <c r="C613" t="n">
+        <v>2385.10009765625</v>
+      </c>
+      <c r="D613" t="n">
+        <v>2285.39990234375</v>
+      </c>
+      <c r="E613" t="n">
+        <v>2305.199951171875</v>
+      </c>
+      <c r="F613" t="n">
+        <v>2305.199951171875</v>
+      </c>
+      <c r="G613" t="n">
+        <v>269</v>
+      </c>
+      <c r="H613" t="n">
+        <v>0.04362483572798542</v>
+      </c>
+      <c r="I613" t="n">
+        <v>-0.03138785421114128</v>
+      </c>
+      <c r="J613" t="n">
+        <v>967.7999877929688</v>
+      </c>
+      <c r="K613" t="n">
+        <v>967.7999877929688</v>
+      </c>
+      <c r="L613" t="n">
+        <v>967.7999877929688</v>
+      </c>
+      <c r="M613" t="n">
+        <v>967.7999877929688</v>
+      </c>
+      <c r="N613" t="n">
+        <v>967.7999877929688</v>
+      </c>
+      <c r="O613" t="n">
+        <v>25</v>
+      </c>
+      <c r="P613" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q613" t="n">
+        <v>0</v>
+      </c>
+      <c r="R613" t="n">
+        <v>4.559999942779541</v>
+      </c>
+      <c r="S613" t="n">
+        <v>4.559999942779541</v>
+      </c>
+      <c r="T613" t="n">
+        <v>4.479499816894531</v>
+      </c>
+      <c r="U613" t="n">
+        <v>4.494500160217285</v>
+      </c>
+      <c r="V613" t="n">
+        <v>4.494500160217285</v>
+      </c>
+      <c r="W613" t="n">
+        <v>398</v>
+      </c>
+      <c r="X613" t="n">
+        <v>0.01797078450174321</v>
+      </c>
+      <c r="Y613" t="n">
+        <v>-0.01436398758424777</v>
+      </c>
+      <c r="Z613" t="n">
+        <v>75.66999816894531</v>
+      </c>
+      <c r="AA613" t="n">
+        <v>76.25</v>
+      </c>
+      <c r="AB613" t="n">
+        <v>75.20999908447266</v>
+      </c>
+      <c r="AC613" t="n">
+        <v>75.52999877929688</v>
+      </c>
+      <c r="AD613" t="n">
+        <v>75.52999877929688</v>
+      </c>
+      <c r="AE613" t="n">
+        <v>280253</v>
+      </c>
+      <c r="AF613" t="n">
+        <v>0.01382796075238957</v>
+      </c>
+      <c r="AG613" t="n">
+        <v>-0.001850130739211419</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" s="2" t="n">
+        <v>45453</v>
+      </c>
+      <c r="B614" t="n">
+        <v>2290.60009765625</v>
+      </c>
+      <c r="C614" t="n">
+        <v>2309.300048828125</v>
+      </c>
+      <c r="D614" t="n">
+        <v>2290.5</v>
+      </c>
+      <c r="E614" t="n">
+        <v>2307.699951171875</v>
+      </c>
+      <c r="F614" t="n">
+        <v>2307.699951171875</v>
+      </c>
+      <c r="G614" t="n">
+        <v>269</v>
+      </c>
+      <c r="H614" t="n">
+        <v>0.008207836205249945</v>
+      </c>
+      <c r="I614" t="n">
+        <v>0.007465228667859409</v>
+      </c>
+      <c r="J614" t="n">
+        <v>972.5</v>
+      </c>
+      <c r="K614" t="n">
+        <v>972.5</v>
+      </c>
+      <c r="L614" t="n">
+        <v>972.5</v>
+      </c>
+      <c r="M614" t="n">
+        <v>972.5</v>
+      </c>
+      <c r="N614" t="n">
+        <v>972.5</v>
+      </c>
+      <c r="O614" t="n">
+        <v>25</v>
+      </c>
+      <c r="P614" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q614" t="n">
+        <v>0</v>
+      </c>
+      <c r="R614" t="n">
+        <v>4.474999904632568</v>
+      </c>
+      <c r="S614" t="n">
+        <v>4.568999767303467</v>
+      </c>
+      <c r="T614" t="n">
+        <v>4.474999904632568</v>
+      </c>
+      <c r="U614" t="n">
+        <v>4.55649995803833</v>
+      </c>
+      <c r="V614" t="n">
+        <v>4.55649995803833</v>
+      </c>
+      <c r="W614" t="n">
+        <v>398</v>
+      </c>
+      <c r="X614" t="n">
+        <v>0.02100555635176411</v>
+      </c>
+      <c r="Y614" t="n">
+        <v>0.01821230282516699</v>
+      </c>
+      <c r="Z614" t="n">
+        <v>75.34999847412109</v>
+      </c>
+      <c r="AA614" t="n">
+        <v>78.29000091552734</v>
+      </c>
+      <c r="AB614" t="n">
+        <v>75.23000335693359</v>
+      </c>
+      <c r="AC614" t="n">
+        <v>77.73999786376953</v>
+      </c>
+      <c r="AD614" t="n">
+        <v>77.73999786376953</v>
+      </c>
+      <c r="AE614" t="n">
+        <v>280253</v>
+      </c>
+      <c r="AF614" t="n">
+        <v>0.04067522826066343</v>
+      </c>
+      <c r="AG614" t="n">
+        <v>0.03171863885928652</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="2" t="n">
+        <v>45456</v>
+      </c>
+      <c r="B615" t="n">
+        <v>2340.89990234375</v>
+      </c>
+      <c r="C615" t="n">
+        <v>2341.300048828125</v>
+      </c>
+      <c r="D615" t="n">
+        <v>2323.800048828125</v>
+      </c>
+      <c r="E615" t="n">
+        <v>2328.199951171875</v>
+      </c>
+      <c r="F615" t="n">
+        <v>2328.199951171875</v>
+      </c>
+      <c r="G615" t="n">
+        <v>22187</v>
+      </c>
+      <c r="H615" t="n">
+        <v>0.007530768410485712</v>
+      </c>
+      <c r="I615" t="n">
+        <v>-0.005425243155061686</v>
+      </c>
+      <c r="J615" t="n">
+        <v>964.5</v>
+      </c>
+      <c r="K615" t="n">
+        <v>965.5</v>
+      </c>
+      <c r="L615" t="n">
+        <v>951</v>
+      </c>
+      <c r="M615" t="n">
+        <v>951.2000122070312</v>
+      </c>
+      <c r="N615" t="n">
+        <v>951.2000122070312</v>
+      </c>
+      <c r="O615" t="n">
+        <v>3289</v>
+      </c>
+      <c r="P615" t="n">
+        <v>0.01524710830704522</v>
+      </c>
+      <c r="Q615" t="n">
+        <v>-0.01378951559664982</v>
+      </c>
+      <c r="R615" t="n">
+        <v>4.533500194549561</v>
+      </c>
+      <c r="S615" t="n">
+        <v>4.539999961853027</v>
+      </c>
+      <c r="T615" t="n">
+        <v>4.490499973297119</v>
+      </c>
+      <c r="U615" t="n">
+        <v>4.506499767303467</v>
+      </c>
+      <c r="V615" t="n">
+        <v>4.506499767303467</v>
+      </c>
+      <c r="W615" t="n">
+        <v>7811</v>
+      </c>
+      <c r="X615" t="n">
+        <v>0.01102326886766757</v>
+      </c>
+      <c r="Y615" t="n">
+        <v>-0.00595575738114123</v>
+      </c>
+      <c r="Z615" t="n">
+        <v>78.37000274658203</v>
+      </c>
+      <c r="AA615" t="n">
+        <v>78.40000152587891</v>
+      </c>
+      <c r="AB615" t="n">
+        <v>78.06999969482422</v>
+      </c>
+      <c r="AC615" t="n">
+        <v>78.30000305175781</v>
+      </c>
+      <c r="AD615" t="n">
+        <v>78.30000305175781</v>
+      </c>
+      <c r="AE615" t="n">
+        <v>9183</v>
+      </c>
+      <c r="AF615" t="n">
+        <v>0.004226999261491806</v>
+      </c>
+      <c r="AG615" t="n">
+        <v>-0.0008931950028197704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>